<commit_message>
17 02 2025 02:00 AM Commit after extent report screenshot attachment s01
</commit_message>
<xml_diff>
--- a/src/test/java/nnd/TestData/TestData.xlsx
+++ b/src/test/java/nnd/TestData/TestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhane\eclipse-workspace\DemoBlazeDataDriven14022025\src\test\java\nnd\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217A3CF3-F114-4B48-B40C-B1F532175400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13C69F7-CBD6-4C25-B7CD-E52ED47CD32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="1188" windowWidth="17280" windowHeight="8880" xr2:uid="{9B67BCA4-154D-493C-AABA-840BFB8F5DE0}"/>
+    <workbookView xWindow="3072" yWindow="1188" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{9B67BCA4-154D-493C-AABA-840BFB8F5DE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -51,16 +51,25 @@
     <t>dhan@01</t>
   </si>
   <si>
-    <t>dhan0102</t>
-  </si>
-  <si>
-    <t>dhan600010</t>
-  </si>
-  <si>
     <t>dhan01</t>
   </si>
   <si>
     <t>dhan6000</t>
+  </si>
+  <si>
+    <t>dhanINV01</t>
+  </si>
+  <si>
+    <t>dhanINV02</t>
+  </si>
+  <si>
+    <t>dhanINV#01</t>
+  </si>
+  <si>
+    <t>dhanINV#02</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -460,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449C7ACF-66E2-407F-89E4-A43DC50F7D0C}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +489,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -488,7 +497,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -505,60 +514,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30D9666-B509-48BB-B569-9E2274A7CB58}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{5F0F683D-DC1E-4522-A171-D76686392BA7}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{A3271673-F453-475F-8006-59760EF6CDE2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17 02 2025 04:48 AM Normal Commit after all 7 testcases pass
</commit_message>
<xml_diff>
--- a/src/test/java/nnd/TestData/TestData.xlsx
+++ b/src/test/java/nnd/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhane\eclipse-workspace\DemoBlazeDataDriven14022025\src\test\java\nnd\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13C69F7-CBD6-4C25-B7CD-E52ED47CD32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157250D2-4F68-417D-A271-E1C1A8555B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="1188" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{9B67BCA4-154D-493C-AABA-840BFB8F5DE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9B67BCA4-154D-493C-AABA-840BFB8F5DE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,19 +57,19 @@
     <t>dhan6000</t>
   </si>
   <si>
-    <t>dhanINV01</t>
-  </si>
-  <si>
-    <t>dhanINV02</t>
-  </si>
-  <si>
-    <t>dhanINV#01</t>
-  </si>
-  <si>
-    <t>dhanINV#02</t>
-  </si>
-  <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>dhan0001</t>
+  </si>
+  <si>
+    <t>dhan0002</t>
+  </si>
+  <si>
+    <t>dhan#0001</t>
+  </si>
+  <si>
+    <t>dhan#0002</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,23 +531,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>